<commit_message>
report new conditions in admin user page
</commit_message>
<xml_diff>
--- a/7RSuperMarket/src/main/resources/Test_Data.xlsx
+++ b/7RSuperMarket/src/main/resources/Test_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18744" windowHeight="9156" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13668" windowHeight="6828" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Page" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="Manage_Category" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:S30"/>
+  <oleSize ref="A1:F21"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>username</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Ring</t>
+  </si>
+  <si>
+    <t>test@123</t>
   </si>
 </sst>
 </file>
@@ -481,10 +484,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,9 +530,18 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -623,7 +635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>